<commit_message>
Restoration et recuperation Argos
</commit_message>
<xml_diff>
--- a/Résultat_test.xlsx
+++ b/Résultat_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburkhart\PycharmProjects\TEST_WEB_CRAWLER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1262FB7-CF85-47CC-B0D4-069E5A022529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9116E6EF-ACCB-441E-9DD5-BDA000DFA35E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{A914211A-8EB7-49ED-87C4-66C4AF9E807E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>selenium</t>
   </si>
@@ -114,9 +114,6 @@
     <t>durée de recherche du script</t>
   </si>
   <si>
-    <t>21 sec</t>
-  </si>
-  <si>
     <t>ARGOS LAB</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>scrapy_selenium</t>
+  </si>
+  <si>
+    <t>0:02:15.328764 (code final)</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,10 +573,10 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,15 +639,12 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>2</v>

</xml_diff>

<commit_message>
get info + excel
</commit_message>
<xml_diff>
--- a/Résultat_test.xlsx
+++ b/Résultat_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburkhart\PycharmProjects\TEST_WEB_CRAWLER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburkhart\Documents\TEST_WEB_CRAWLER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1262FB7-CF85-47CC-B0D4-069E5A022529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9618B3FD-09B1-475C-9A6B-6ECAC539B2F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{A914211A-8EB7-49ED-87C4-66C4AF9E807E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A914211A-8EB7-49ED-87C4-66C4AF9E807E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>selenium</t>
   </si>
@@ -111,12 +111,6 @@
     <t xml:space="preserve">boucle while </t>
   </si>
   <si>
-    <t>durée de recherche du script</t>
-  </si>
-  <si>
-    <t>21 sec</t>
-  </si>
-  <si>
     <t>ARGOS LAB</t>
   </si>
   <si>
@@ -129,13 +123,40 @@
     <t xml:space="preserve">3 h </t>
   </si>
   <si>
-    <t>difficulté (intuitivité) 1 a 3</t>
-  </si>
-  <si>
-    <t>20 min (fais avec detection mouvement)</t>
-  </si>
-  <si>
     <t>scrapy_selenium</t>
+  </si>
+  <si>
+    <t>IUPATH</t>
+  </si>
+  <si>
+    <t>temps de recherche web</t>
+  </si>
+  <si>
+    <t>1 h (6h sans les tests)</t>
+  </si>
+  <si>
+    <t>0 h</t>
+  </si>
+  <si>
+    <t>4 h</t>
+  </si>
+  <si>
+    <t>difficulté (intuitivité) 1 a 4</t>
+  </si>
+  <si>
+    <t>20 (fais avec detection mouvement)</t>
+  </si>
+  <si>
+    <t>31 sec</t>
+  </si>
+  <si>
+    <t>2 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">durée de recherche du script (une information) </t>
+  </si>
+  <si>
+    <t>15 sec</t>
   </si>
 </sst>
 </file>
@@ -487,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89092D9-7D3A-490E-8CD8-D720EE3E8598}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +522,7 @@
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -515,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -529,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -543,7 +564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -554,7 +575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -565,7 +586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -573,13 +594,16 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -589,8 +613,11 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -598,10 +625,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -609,10 +639,13 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -620,10 +653,13 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -631,29 +667,52 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -662,6 +721,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F2C878D8776BA4E97EE4AD2EAF5C104" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99de6405519137be15b7b139d1491bc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d782a7ddadf744fc5d4ce9623e820201">
     <xsd:element name="properties">
@@ -775,22 +849,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84B3901-92BE-4975-AAF7-49130A5FDA9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98823BB0-B821-498A-B8DD-417729FDF7EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D84A165-79EE-42C9-9E05-A197798E7290}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -804,27 +886,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98823BB0-B821-498A-B8DD-417729FDF7EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84B3901-92BE-4975-AAF7-49130A5FDA9A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>